<commit_message>
Ghoast in the Excel
</commit_message>
<xml_diff>
--- a/Ghoast.xlsx
+++ b/Ghoast.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aphrodite\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D09ADE-C7F5-4724-B122-5F8CBC207A68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8737AECE-8431-40E8-B906-9016C676EB3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{488E0E3E-739F-4D2D-ADDE-9D5CCFF1FC31}"/>
+    <workbookView xWindow="3660" yWindow="4275" windowWidth="21600" windowHeight="12735" xr2:uid="{488E0E3E-739F-4D2D-ADDE-9D5CCFF1FC31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Data</t>
     <phoneticPr fontId="1"/>
@@ -135,17 +135,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color theme="9"/>
-      </right>
-      <top style="medium">
-        <color theme="9"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color theme="9"/>
       </left>
@@ -187,13 +176,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -212,13 +210,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
@@ -541,7 +542,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -550,71 +551,77 @@
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" s="9" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>123</v>
       </c>
-      <c r="E2" s="7" t="str">
+      <c r="E2" s="6" t="str">
         <f>D2&amp;""</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>456</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>789</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>1112</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>1314</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>